<commit_message>
Update BinaryFiles to support adding python38.zip to the package Updates to example files in inst/extdata Various StandViz.py updates
</commit_message>
<xml_diff>
--- a/inst/extdata/SouthernPine.xlsx
+++ b/inst/extdata/SouthernPine.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mccarterj\McCarter\Projects\rSVS\inst\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mccarterj\McCarter\Projects\rSVS\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,12 +36,6 @@
     <t>Height</t>
   </si>
   <si>
-    <t>CRadius1</t>
-  </si>
-  <si>
-    <t>CRatio1</t>
-  </si>
-  <si>
     <t>TPA</t>
   </si>
   <si>
@@ -70,6 +64,12 @@
   </si>
   <si>
     <t>Live/Dead</t>
+  </si>
+  <si>
+    <t>Cradius</t>
+  </si>
+  <si>
+    <t>Cratio</t>
   </si>
 </sst>
 </file>
@@ -879,7 +879,7 @@
   <dimension ref="A1:N195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,27 +892,27 @@
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -927,30 +927,30 @@
         <v>4</v>
       </c>
       <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>2000</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -988,13 +988,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>2000</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>101</v>
@@ -1032,13 +1032,13 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>2000</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>102</v>
@@ -1076,13 +1076,13 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>2000</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>103</v>
@@ -1120,13 +1120,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>2000</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>104</v>
@@ -1164,13 +1164,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>2000</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>105</v>
@@ -1208,13 +1208,13 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>2000</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>106</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>2000</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>107</v>
@@ -1296,13 +1296,13 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>2000</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>108</v>
@@ -1340,13 +1340,13 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>2000</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <v>109</v>
@@ -1384,13 +1384,13 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>2000</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <v>110</v>
@@ -1428,13 +1428,13 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>2000</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <v>111</v>
@@ -1472,13 +1472,13 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>2000</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>112</v>
@@ -1516,13 +1516,13 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>2000</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D15">
         <v>113</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16">
         <v>2000</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D16">
         <v>114</v>
@@ -1604,13 +1604,13 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17">
         <v>2000</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D17">
         <v>201</v>
@@ -1648,13 +1648,13 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18">
         <v>2000</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D18">
         <v>202</v>
@@ -1692,13 +1692,13 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B19">
         <v>2000</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <v>203</v>
@@ -1736,13 +1736,13 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B20">
         <v>2000</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D20">
         <v>204</v>
@@ -1780,13 +1780,13 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>2000</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D21">
         <v>205</v>
@@ -1824,13 +1824,13 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B22">
         <v>2000</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>206</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B23">
         <v>2000</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D23">
         <v>207</v>
@@ -1912,13 +1912,13 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B24">
         <v>2000</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D24">
         <v>208</v>
@@ -1956,13 +1956,13 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B25">
         <v>2000</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D25">
         <v>209</v>
@@ -2000,13 +2000,13 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B26">
         <v>2000</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D26">
         <v>210</v>
@@ -2044,13 +2044,13 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B27">
         <v>2000</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D27">
         <v>211</v>
@@ -2088,13 +2088,13 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B28">
         <v>2000</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D28">
         <v>212</v>
@@ -2132,13 +2132,13 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B29">
         <v>2000</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D29">
         <v>213</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B30">
         <v>2000</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D30">
         <v>214</v>
@@ -2220,13 +2220,13 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B31">
         <v>2000</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D31">
         <v>215</v>
@@ -2264,13 +2264,13 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B32">
         <v>2000</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D32">
         <v>301</v>
@@ -2308,13 +2308,13 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B33">
         <v>2000</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D33">
         <v>302</v>
@@ -2352,13 +2352,13 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B34">
         <v>2000</v>
       </c>
       <c r="C34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D34">
         <v>303</v>
@@ -2396,13 +2396,13 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B35">
         <v>2000</v>
       </c>
       <c r="C35" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D35">
         <v>304</v>
@@ -2440,13 +2440,13 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B36">
         <v>2000</v>
       </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D36">
         <v>305</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B37">
         <v>2000</v>
       </c>
       <c r="C37" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D37">
         <v>306</v>
@@ -2528,13 +2528,13 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B38">
         <v>2000</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D38">
         <v>307</v>
@@ -2572,13 +2572,13 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B39">
         <v>2000</v>
       </c>
       <c r="C39" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D39">
         <v>308</v>
@@ -2616,13 +2616,13 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B40">
         <v>2000</v>
       </c>
       <c r="C40" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D40">
         <v>309</v>
@@ -2660,13 +2660,13 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B41">
         <v>2000</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D41">
         <v>310</v>
@@ -2704,13 +2704,13 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B42">
         <v>2000</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D42">
         <v>311</v>
@@ -2748,13 +2748,13 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B43">
         <v>2000</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D43">
         <v>312</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B44">
         <v>2000</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D44">
         <v>313</v>
@@ -2836,13 +2836,13 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B45">
         <v>2000</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D45">
         <v>314</v>
@@ -2880,13 +2880,13 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B46">
         <v>2000</v>
       </c>
       <c r="C46" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D46">
         <v>315</v>
@@ -2924,13 +2924,13 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B47">
         <v>2000</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D47">
         <v>401</v>
@@ -2968,13 +2968,13 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B48">
         <v>2000</v>
       </c>
       <c r="C48" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D48">
         <v>402</v>
@@ -3012,13 +3012,13 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B49">
         <v>2000</v>
       </c>
       <c r="C49" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D49">
         <v>403</v>
@@ -3056,13 +3056,13 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B50">
         <v>2000</v>
       </c>
       <c r="C50" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D50">
         <v>404</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B51">
         <v>2000</v>
       </c>
       <c r="C51" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D51">
         <v>405</v>
@@ -3144,13 +3144,13 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B52">
         <v>2000</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D52">
         <v>406</v>
@@ -3188,13 +3188,13 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B53">
         <v>2000</v>
       </c>
       <c r="C53" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D53">
         <v>407</v>
@@ -3232,13 +3232,13 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B54">
         <v>2000</v>
       </c>
       <c r="C54" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D54">
         <v>408</v>
@@ -3276,13 +3276,13 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B55">
         <v>2000</v>
       </c>
       <c r="C55" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D55">
         <v>409</v>
@@ -3320,13 +3320,13 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B56">
         <v>2000</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D56">
         <v>410</v>
@@ -3364,13 +3364,13 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B57">
         <v>2000</v>
       </c>
       <c r="C57" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D57">
         <v>411</v>
@@ -3408,13 +3408,13 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B58">
         <v>2000</v>
       </c>
       <c r="C58" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D58">
         <v>412</v>
@@ -3452,13 +3452,13 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B59">
         <v>2000</v>
       </c>
       <c r="C59" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D59">
         <v>413</v>
@@ -3496,13 +3496,13 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B60">
         <v>2000</v>
       </c>
       <c r="C60" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D60">
         <v>414</v>
@@ -3540,13 +3540,13 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B61">
         <v>2000</v>
       </c>
       <c r="C61" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D61">
         <v>415</v>
@@ -3584,13 +3584,13 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B62">
         <v>2000</v>
       </c>
       <c r="C62" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D62">
         <v>501</v>
@@ -3628,13 +3628,13 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B63">
         <v>2000</v>
       </c>
       <c r="C63" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D63">
         <v>502</v>
@@ -3672,13 +3672,13 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B64">
         <v>2000</v>
       </c>
       <c r="C64" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D64">
         <v>503</v>
@@ -3716,13 +3716,13 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B65">
         <v>2000</v>
       </c>
       <c r="C65" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D65">
         <v>504</v>
@@ -3760,13 +3760,13 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B66">
         <v>2000</v>
       </c>
       <c r="C66" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D66">
         <v>505</v>
@@ -3804,13 +3804,13 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B67">
         <v>2000</v>
       </c>
       <c r="C67" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D67">
         <v>506</v>
@@ -3848,13 +3848,13 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B68">
         <v>2000</v>
       </c>
       <c r="C68" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D68">
         <v>507</v>
@@ -3892,13 +3892,13 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B69">
         <v>2000</v>
       </c>
       <c r="C69" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D69">
         <v>508</v>
@@ -3936,13 +3936,13 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B70">
         <v>2000</v>
       </c>
       <c r="C70" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D70">
         <v>509</v>
@@ -3980,13 +3980,13 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B71">
         <v>2000</v>
       </c>
       <c r="C71" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D71">
         <v>510</v>
@@ -4024,13 +4024,13 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B72">
         <v>2000</v>
       </c>
       <c r="C72" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D72">
         <v>511</v>
@@ -4068,13 +4068,13 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B73">
         <v>2000</v>
       </c>
       <c r="C73" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D73">
         <v>512</v>
@@ -4112,13 +4112,13 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B74">
         <v>2000</v>
       </c>
       <c r="C74" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D74">
         <v>513</v>
@@ -4156,13 +4156,13 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B75">
         <v>2000</v>
       </c>
       <c r="C75" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D75">
         <v>514</v>
@@ -4200,13 +4200,13 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B76">
         <v>2000</v>
       </c>
       <c r="C76" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D76">
         <v>515</v>
@@ -4244,13 +4244,13 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B77">
         <v>2000</v>
       </c>
       <c r="C77" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D77">
         <v>601</v>
@@ -4288,13 +4288,13 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B78">
         <v>2000</v>
       </c>
       <c r="C78" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D78">
         <v>602</v>
@@ -4332,13 +4332,13 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B79">
         <v>2000</v>
       </c>
       <c r="C79" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D79">
         <v>603</v>
@@ -4376,13 +4376,13 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B80">
         <v>2000</v>
       </c>
       <c r="C80" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D80">
         <v>604</v>
@@ -4420,13 +4420,13 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B81">
         <v>2000</v>
       </c>
       <c r="C81" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D81">
         <v>605</v>
@@ -4464,13 +4464,13 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B82">
         <v>2000</v>
       </c>
       <c r="C82" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D82">
         <v>606</v>
@@ -4508,13 +4508,13 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B83">
         <v>2000</v>
       </c>
       <c r="C83" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D83">
         <v>607</v>
@@ -4552,13 +4552,13 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B84">
         <v>2000</v>
       </c>
       <c r="C84" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D84">
         <v>608</v>
@@ -4596,13 +4596,13 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B85">
         <v>2000</v>
       </c>
       <c r="C85" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D85">
         <v>609</v>
@@ -4640,13 +4640,13 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B86">
         <v>2000</v>
       </c>
       <c r="C86" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D86">
         <v>610</v>
@@ -4684,13 +4684,13 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B87">
         <v>2000</v>
       </c>
       <c r="C87" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D87">
         <v>611</v>
@@ -4728,13 +4728,13 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B88">
         <v>2000</v>
       </c>
       <c r="C88" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D88">
         <v>612</v>
@@ -4772,13 +4772,13 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B89">
         <v>2000</v>
       </c>
       <c r="C89" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D89">
         <v>613</v>
@@ -4816,13 +4816,13 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B90">
         <v>2000</v>
       </c>
       <c r="C90" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D90">
         <v>614</v>
@@ -4860,13 +4860,13 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B91">
         <v>2000</v>
       </c>
       <c r="C91" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D91">
         <v>615</v>
@@ -4904,13 +4904,13 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B92">
         <v>2000</v>
       </c>
       <c r="C92" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D92">
         <v>701</v>
@@ -4948,13 +4948,13 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B93">
         <v>2000</v>
       </c>
       <c r="C93" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D93">
         <v>702</v>
@@ -4992,13 +4992,13 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B94">
         <v>2000</v>
       </c>
       <c r="C94" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D94">
         <v>703</v>
@@ -5036,13 +5036,13 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B95">
         <v>2000</v>
       </c>
       <c r="C95" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D95">
         <v>704</v>
@@ -5080,13 +5080,13 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B96">
         <v>2000</v>
       </c>
       <c r="C96" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D96">
         <v>705</v>
@@ -5124,13 +5124,13 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B97">
         <v>2000</v>
       </c>
       <c r="C97" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D97">
         <v>706</v>
@@ -5168,13 +5168,13 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B98">
         <v>2000</v>
       </c>
       <c r="C98" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D98">
         <v>707</v>
@@ -5212,13 +5212,13 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B99">
         <v>2000</v>
       </c>
       <c r="C99" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D99">
         <v>708</v>
@@ -5256,13 +5256,13 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B100">
         <v>2000</v>
       </c>
       <c r="C100" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D100">
         <v>709</v>
@@ -5300,13 +5300,13 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B101">
         <v>2000</v>
       </c>
       <c r="C101" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D101">
         <v>710</v>
@@ -5344,13 +5344,13 @@
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B102">
         <v>2000</v>
       </c>
       <c r="C102" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D102">
         <v>711</v>
@@ -5388,13 +5388,13 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B103">
         <v>2000</v>
       </c>
       <c r="C103" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D103">
         <v>712</v>
@@ -5432,13 +5432,13 @@
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B104">
         <v>2000</v>
       </c>
       <c r="C104" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D104">
         <v>713</v>
@@ -5476,13 +5476,13 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B105">
         <v>2000</v>
       </c>
       <c r="C105" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D105">
         <v>714</v>
@@ -5520,13 +5520,13 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B106">
         <v>2000</v>
       </c>
       <c r="C106" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D106">
         <v>715</v>
@@ -5564,13 +5564,13 @@
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B107">
         <v>2000</v>
       </c>
       <c r="C107" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D107">
         <v>801</v>
@@ -5608,13 +5608,13 @@
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B108">
         <v>2000</v>
       </c>
       <c r="C108" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D108">
         <v>802</v>
@@ -5652,13 +5652,13 @@
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B109">
         <v>2000</v>
       </c>
       <c r="C109" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D109">
         <v>803</v>
@@ -5696,13 +5696,13 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B110">
         <v>2000</v>
       </c>
       <c r="C110" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D110">
         <v>804</v>
@@ -5740,13 +5740,13 @@
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B111">
         <v>2000</v>
       </c>
       <c r="C111" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D111">
         <v>805</v>
@@ -5784,13 +5784,13 @@
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B112">
         <v>2000</v>
       </c>
       <c r="C112" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D112">
         <v>806</v>
@@ -5828,13 +5828,13 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B113">
         <v>2000</v>
       </c>
       <c r="C113" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D113">
         <v>807</v>
@@ -5872,13 +5872,13 @@
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B114">
         <v>2000</v>
       </c>
       <c r="C114" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D114">
         <v>808</v>
@@ -5916,13 +5916,13 @@
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B115">
         <v>2000</v>
       </c>
       <c r="C115" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D115">
         <v>809</v>
@@ -5960,13 +5960,13 @@
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B116">
         <v>2000</v>
       </c>
       <c r="C116" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D116">
         <v>810</v>
@@ -6004,13 +6004,13 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B117">
         <v>2000</v>
       </c>
       <c r="C117" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D117">
         <v>811</v>
@@ -6048,13 +6048,13 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B118">
         <v>2000</v>
       </c>
       <c r="C118" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D118">
         <v>812</v>
@@ -6092,13 +6092,13 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B119">
         <v>2000</v>
       </c>
       <c r="C119" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D119">
         <v>813</v>
@@ -6136,13 +6136,13 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B120">
         <v>2000</v>
       </c>
       <c r="C120" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D120">
         <v>814</v>
@@ -6180,13 +6180,13 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B121">
         <v>2000</v>
       </c>
       <c r="C121" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D121">
         <v>815</v>
@@ -6224,13 +6224,13 @@
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B122">
         <v>2000</v>
       </c>
       <c r="C122" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D122">
         <v>901</v>
@@ -6268,13 +6268,13 @@
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B123">
         <v>2000</v>
       </c>
       <c r="C123" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D123">
         <v>902</v>
@@ -6312,13 +6312,13 @@
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B124">
         <v>2000</v>
       </c>
       <c r="C124" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D124">
         <v>903</v>
@@ -6356,13 +6356,13 @@
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B125">
         <v>2000</v>
       </c>
       <c r="C125" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D125">
         <v>904</v>
@@ -6400,13 +6400,13 @@
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B126">
         <v>2000</v>
       </c>
       <c r="C126" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D126">
         <v>905</v>
@@ -6444,13 +6444,13 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B127">
         <v>2000</v>
       </c>
       <c r="C127" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D127">
         <v>906</v>
@@ -6488,13 +6488,13 @@
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B128">
         <v>2000</v>
       </c>
       <c r="C128" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D128">
         <v>907</v>
@@ -6532,13 +6532,13 @@
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B129">
         <v>2000</v>
       </c>
       <c r="C129" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D129">
         <v>908</v>
@@ -6576,13 +6576,13 @@
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B130">
         <v>2000</v>
       </c>
       <c r="C130" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D130">
         <v>909</v>
@@ -6620,13 +6620,13 @@
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B131">
         <v>2000</v>
       </c>
       <c r="C131" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D131">
         <v>910</v>
@@ -6664,13 +6664,13 @@
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B132">
         <v>2000</v>
       </c>
       <c r="C132" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D132">
         <v>911</v>
@@ -6708,13 +6708,13 @@
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B133">
         <v>2000</v>
       </c>
       <c r="C133" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D133">
         <v>912</v>
@@ -6752,13 +6752,13 @@
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B134">
         <v>2000</v>
       </c>
       <c r="C134" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D134">
         <v>1001</v>
@@ -6796,13 +6796,13 @@
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B135">
         <v>2000</v>
       </c>
       <c r="C135" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D135">
         <v>1002</v>
@@ -6840,13 +6840,13 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B136">
         <v>2000</v>
       </c>
       <c r="C136" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D136">
         <v>1003</v>
@@ -6884,13 +6884,13 @@
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B137">
         <v>2000</v>
       </c>
       <c r="C137" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D137">
         <v>1004</v>
@@ -6928,13 +6928,13 @@
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B138">
         <v>2000</v>
       </c>
       <c r="C138" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D138">
         <v>1005</v>
@@ -6972,13 +6972,13 @@
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B139">
         <v>2000</v>
       </c>
       <c r="C139" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D139">
         <v>1006</v>
@@ -7016,13 +7016,13 @@
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B140">
         <v>2000</v>
       </c>
       <c r="C140" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D140">
         <v>1007</v>
@@ -7060,13 +7060,13 @@
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B141">
         <v>2000</v>
       </c>
       <c r="C141" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D141">
         <v>1008</v>
@@ -7104,13 +7104,13 @@
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B142">
         <v>2000</v>
       </c>
       <c r="C142" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D142">
         <v>1009</v>
@@ -7148,13 +7148,13 @@
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B143">
         <v>2000</v>
       </c>
       <c r="C143" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D143">
         <v>1010</v>
@@ -7192,13 +7192,13 @@
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B144">
         <v>2000</v>
       </c>
       <c r="C144" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D144">
         <v>1011</v>
@@ -7236,13 +7236,13 @@
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B145">
         <v>2000</v>
       </c>
       <c r="C145" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D145">
         <v>1101</v>
@@ -7280,13 +7280,13 @@
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B146">
         <v>2000</v>
       </c>
       <c r="C146" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D146">
         <v>1102</v>
@@ -7324,13 +7324,13 @@
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B147">
         <v>2000</v>
       </c>
       <c r="C147" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D147">
         <v>1103</v>
@@ -7368,13 +7368,13 @@
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B148">
         <v>2000</v>
       </c>
       <c r="C148" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D148">
         <v>1104</v>
@@ -7412,13 +7412,13 @@
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B149">
         <v>2000</v>
       </c>
       <c r="C149" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D149">
         <v>1105</v>
@@ -7456,13 +7456,13 @@
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B150">
         <v>2000</v>
       </c>
       <c r="C150" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D150">
         <v>1106</v>
@@ -7500,13 +7500,13 @@
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B151">
         <v>2000</v>
       </c>
       <c r="C151" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D151">
         <v>1107</v>
@@ -7544,13 +7544,13 @@
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B152">
         <v>2000</v>
       </c>
       <c r="C152" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D152">
         <v>1108</v>
@@ -7588,13 +7588,13 @@
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B153">
         <v>2000</v>
       </c>
       <c r="C153" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D153">
         <v>1109</v>
@@ -7632,13 +7632,13 @@
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B154">
         <v>2000</v>
       </c>
       <c r="C154" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D154">
         <v>1201</v>
@@ -7676,13 +7676,13 @@
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B155">
         <v>2000</v>
       </c>
       <c r="C155" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D155">
         <v>1202</v>
@@ -7720,13 +7720,13 @@
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B156">
         <v>2000</v>
       </c>
       <c r="C156" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D156">
         <v>1203</v>
@@ -7764,13 +7764,13 @@
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B157">
         <v>2000</v>
       </c>
       <c r="C157" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D157">
         <v>1204</v>
@@ -7808,13 +7808,13 @@
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B158">
         <v>2000</v>
       </c>
       <c r="C158" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D158">
         <v>1205</v>
@@ -7852,13 +7852,13 @@
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B159">
         <v>2000</v>
       </c>
       <c r="C159" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D159">
         <v>1206</v>
@@ -7896,13 +7896,13 @@
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B160">
         <v>2000</v>
       </c>
       <c r="C160" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D160">
         <v>1207</v>
@@ -7940,13 +7940,13 @@
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B161">
         <v>2000</v>
       </c>
       <c r="C161" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D161">
         <v>1301</v>
@@ -7984,13 +7984,13 @@
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B162">
         <v>2000</v>
       </c>
       <c r="C162" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D162">
         <v>1302</v>
@@ -8028,13 +8028,13 @@
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B163">
         <v>2000</v>
       </c>
       <c r="C163" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D163">
         <v>1303</v>
@@ -8072,13 +8072,13 @@
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B164">
         <v>2000</v>
       </c>
       <c r="C164" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D164">
         <v>1304</v>
@@ -8116,13 +8116,13 @@
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B165">
         <v>2000</v>
       </c>
       <c r="C165" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D165">
         <v>1305</v>
@@ -8160,13 +8160,13 @@
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B166">
         <v>2000</v>
       </c>
       <c r="C166" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D166">
         <v>1401</v>
@@ -8204,13 +8204,13 @@
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B167">
         <v>2000</v>
       </c>
       <c r="C167" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D167">
         <v>1402</v>
@@ -8248,13 +8248,13 @@
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B168">
         <v>2000</v>
       </c>
       <c r="C168" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D168">
         <v>1403</v>
@@ -8292,13 +8292,13 @@
     </row>
     <row r="169" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B169">
         <v>2000</v>
       </c>
       <c r="C169" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D169">
         <v>1404</v>
@@ -8336,13 +8336,13 @@
     </row>
     <row r="170" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B170">
         <v>2000</v>
       </c>
       <c r="C170" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D170">
         <v>1405</v>
@@ -8380,13 +8380,13 @@
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B171">
         <v>2000</v>
       </c>
       <c r="C171" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D171">
         <v>1406</v>
@@ -8424,13 +8424,13 @@
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B172">
         <v>2000</v>
       </c>
       <c r="C172" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D172">
         <v>1407</v>
@@ -8468,13 +8468,13 @@
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B173">
         <v>2000</v>
       </c>
       <c r="C173" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D173">
         <v>1408</v>
@@ -8512,13 +8512,13 @@
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B174">
         <v>2000</v>
       </c>
       <c r="C174" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D174">
         <v>1409</v>
@@ -8556,13 +8556,13 @@
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B175">
         <v>2000</v>
       </c>
       <c r="C175" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D175">
         <v>1410</v>
@@ -8600,13 +8600,13 @@
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B176">
         <v>2000</v>
       </c>
       <c r="C176" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D176">
         <v>1411</v>
@@ -8644,13 +8644,13 @@
     </row>
     <row r="177" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B177">
         <v>2000</v>
       </c>
       <c r="C177" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D177">
         <v>1412</v>
@@ -8688,13 +8688,13 @@
     </row>
     <row r="178" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B178">
         <v>2000</v>
       </c>
       <c r="C178" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D178">
         <v>1413</v>
@@ -8732,13 +8732,13 @@
     </row>
     <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B179">
         <v>2000</v>
       </c>
       <c r="C179" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D179">
         <v>1414</v>
@@ -8776,13 +8776,13 @@
     </row>
     <row r="180" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B180">
         <v>2000</v>
       </c>
       <c r="C180" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D180">
         <v>1415</v>
@@ -8820,13 +8820,13 @@
     </row>
     <row r="181" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B181">
         <v>2000</v>
       </c>
       <c r="C181" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D181">
         <v>1501</v>
@@ -8864,13 +8864,13 @@
     </row>
     <row r="182" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B182">
         <v>2000</v>
       </c>
       <c r="C182" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D182">
         <v>1502</v>
@@ -8908,13 +8908,13 @@
     </row>
     <row r="183" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B183">
         <v>2000</v>
       </c>
       <c r="C183" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D183">
         <v>1503</v>
@@ -8952,13 +8952,13 @@
     </row>
     <row r="184" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B184">
         <v>2000</v>
       </c>
       <c r="C184" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D184">
         <v>1504</v>
@@ -8996,13 +8996,13 @@
     </row>
     <row r="185" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B185">
         <v>2000</v>
       </c>
       <c r="C185" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D185">
         <v>1505</v>
@@ -9040,13 +9040,13 @@
     </row>
     <row r="186" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B186">
         <v>2000</v>
       </c>
       <c r="C186" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D186">
         <v>1506</v>
@@ -9084,13 +9084,13 @@
     </row>
     <row r="187" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B187">
         <v>2000</v>
       </c>
       <c r="C187" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D187">
         <v>1507</v>
@@ -9128,13 +9128,13 @@
     </row>
     <row r="188" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B188">
         <v>2000</v>
       </c>
       <c r="C188" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D188">
         <v>1508</v>
@@ -9172,13 +9172,13 @@
     </row>
     <row r="189" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B189">
         <v>2000</v>
       </c>
       <c r="C189" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D189">
         <v>1509</v>
@@ -9216,13 +9216,13 @@
     </row>
     <row r="190" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B190">
         <v>2000</v>
       </c>
       <c r="C190" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D190">
         <v>1510</v>
@@ -9260,13 +9260,13 @@
     </row>
     <row r="191" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B191">
         <v>2000</v>
       </c>
       <c r="C191" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D191">
         <v>1511</v>
@@ -9304,13 +9304,13 @@
     </row>
     <row r="192" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B192">
         <v>2000</v>
       </c>
       <c r="C192" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D192">
         <v>1512</v>
@@ -9348,13 +9348,13 @@
     </row>
     <row r="193" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B193">
         <v>2000</v>
       </c>
       <c r="C193" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D193">
         <v>1513</v>
@@ -9392,13 +9392,13 @@
     </row>
     <row r="194" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B194">
         <v>2000</v>
       </c>
       <c r="C194" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D194">
         <v>1514</v>
@@ -9436,13 +9436,13 @@
     </row>
     <row r="195" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B195">
         <v>2000</v>
       </c>
       <c r="C195" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D195">
         <v>1515</v>

</xml_diff>